<commit_message>
Renamng the test ranges
</commit_message>
<xml_diff>
--- a/best_results/individual_feature_analysis/r2/best_r2_WV14_test_range_1.xlsx
+++ b/best_results/individual_feature_analysis/r2/best_r2_WV14_test_range_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legra\WaterRiskML\best_results\individual_feature_analysis\r2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CF68F0-6F7E-4C72-8755-CB76FD5E4161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D216BD-1182-47B8-B90E-57D0C94F20B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3114" yWindow="3114" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.3125" customWidth="1"/>
+    <col min="1" max="1" width="22.62890625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -507,37 +507,37 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>-0.42</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="D2">
-        <v>-0.19</v>
+        <v>-0.47</v>
       </c>
       <c r="E2">
-        <v>-0.18</v>
+        <v>-0.62</v>
       </c>
       <c r="F2">
-        <v>-0.02</v>
+        <v>-0.65</v>
       </c>
       <c r="G2">
-        <v>-0.25</v>
+        <v>-0.36</v>
       </c>
       <c r="H2">
-        <v>-0.1</v>
+        <v>-0.24</v>
       </c>
       <c r="I2">
-        <v>-0.22</v>
+        <v>-0.76</v>
       </c>
       <c r="J2">
-        <v>-0.14000000000000001</v>
+        <v>-0.62</v>
       </c>
       <c r="K2">
-        <v>-0.33</v>
+        <v>-0.34</v>
       </c>
       <c r="L2">
-        <v>-0.2</v>
+        <v>-0.47</v>
       </c>
       <c r="M2">
-        <v>-0.17</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -546,37 +546,37 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>-0.44</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="D3">
-        <v>-0.17</v>
+        <v>-0.46</v>
       </c>
       <c r="E3">
-        <v>-0.14000000000000001</v>
+        <v>-0.6</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-0.64</v>
       </c>
       <c r="G3">
-        <v>-0.19</v>
+        <v>-0.34</v>
       </c>
       <c r="H3">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.25</v>
       </c>
       <c r="I3">
-        <v>-0.17</v>
+        <v>-0.76</v>
       </c>
       <c r="J3">
-        <v>-0.2</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="K3">
-        <v>-0.36</v>
+        <v>-0.34</v>
       </c>
       <c r="L3">
-        <v>-0.18</v>
+        <v>-0.49</v>
       </c>
       <c r="M3">
-        <v>-0.11</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -585,37 +585,37 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>-0.44</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="D4">
-        <v>-0.16</v>
+        <v>-0.46</v>
       </c>
       <c r="E4">
-        <v>-0.13</v>
+        <v>-0.6</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.64</v>
       </c>
       <c r="G4">
-        <v>-0.19</v>
+        <v>-0.35</v>
       </c>
       <c r="H4">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.25</v>
       </c>
       <c r="I4">
-        <v>-0.17</v>
+        <v>-0.76</v>
       </c>
       <c r="J4">
-        <v>-0.2</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="K4">
-        <v>-0.37</v>
+        <v>-0.34</v>
       </c>
       <c r="L4">
-        <v>-0.18</v>
+        <v>-0.49</v>
       </c>
       <c r="M4">
-        <v>-0.09</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -624,37 +624,37 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>-0.44</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="D5">
-        <v>-0.15</v>
+        <v>-0.47</v>
       </c>
       <c r="E5">
-        <v>-0.12</v>
+        <v>-0.6</v>
       </c>
       <c r="F5">
-        <v>-0.02</v>
+        <v>-0.65</v>
       </c>
       <c r="G5">
-        <v>-0.19</v>
+        <v>-0.35</v>
       </c>
       <c r="H5">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.26</v>
       </c>
       <c r="I5">
-        <v>-0.16</v>
+        <v>-0.77</v>
       </c>
       <c r="J5">
-        <v>-0.21</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="K5">
-        <v>-0.38</v>
+        <v>-0.34</v>
       </c>
       <c r="L5">
-        <v>-0.16</v>
+        <v>-0.48</v>
       </c>
       <c r="M5">
-        <v>-0.08</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -665,37 +665,37 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>-0.55000000000000004</v>
+        <v>-0.75</v>
       </c>
       <c r="D6">
-        <v>-0.46</v>
+        <v>-0.52</v>
       </c>
       <c r="E6">
-        <v>-0.62</v>
+        <v>-0.77</v>
       </c>
       <c r="F6">
-        <v>-0.82</v>
+        <v>-0.47</v>
       </c>
       <c r="G6">
-        <v>-0.46</v>
+        <v>-0.48</v>
       </c>
       <c r="H6">
-        <v>0.06</v>
+        <v>-0.63</v>
       </c>
       <c r="I6">
-        <v>-0.52</v>
+        <v>-1.07</v>
       </c>
       <c r="J6">
-        <v>-0.55000000000000004</v>
+        <v>-0.94</v>
       </c>
       <c r="K6">
-        <v>-0.23</v>
+        <v>-0.35</v>
       </c>
       <c r="L6">
-        <v>-0.83</v>
+        <v>-0.61</v>
       </c>
       <c r="M6">
-        <v>-0.46</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -704,37 +704,37 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>-0.55000000000000004</v>
+        <v>-2.6</v>
       </c>
       <c r="D7">
+        <v>-0.52</v>
+      </c>
+      <c r="E7">
+        <v>-0.77</v>
+      </c>
+      <c r="F7">
+        <v>-0.59</v>
+      </c>
+      <c r="G7">
         <v>-0.47</v>
       </c>
-      <c r="E7">
-        <v>-0.62</v>
-      </c>
-      <c r="F7">
-        <v>-1.63</v>
-      </c>
-      <c r="G7">
-        <v>-290.45</v>
-      </c>
       <c r="H7">
-        <v>0.06</v>
+        <v>-1.25</v>
       </c>
       <c r="I7">
-        <v>-0.65</v>
+        <v>-1.07</v>
       </c>
       <c r="J7">
-        <v>-0.55000000000000004</v>
+        <v>-0.94</v>
       </c>
       <c r="K7">
-        <v>-0.23</v>
+        <v>-0.35</v>
       </c>
       <c r="L7">
-        <v>-0.83</v>
+        <v>-0.61</v>
       </c>
       <c r="M7">
-        <v>-0.46</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -743,37 +743,37 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>-0.55000000000000004</v>
+        <v>-1.9</v>
       </c>
       <c r="D8">
+        <v>-0.52</v>
+      </c>
+      <c r="E8">
+        <v>-0.77</v>
+      </c>
+      <c r="F8">
+        <v>-0.89</v>
+      </c>
+      <c r="G8">
         <v>-0.47</v>
       </c>
-      <c r="E8">
-        <v>-0.62</v>
-      </c>
-      <c r="F8">
-        <v>-0.82</v>
-      </c>
-      <c r="G8">
-        <v>-268.12</v>
-      </c>
       <c r="H8">
-        <v>0.06</v>
+        <v>-0.31</v>
       </c>
       <c r="I8">
-        <v>-0.65</v>
+        <v>-1.07</v>
       </c>
       <c r="J8">
-        <v>-0.55000000000000004</v>
+        <v>-0.94</v>
       </c>
       <c r="K8">
-        <v>-0.23</v>
+        <v>-0.35</v>
       </c>
       <c r="L8">
-        <v>-0.83</v>
+        <v>-0.61</v>
       </c>
       <c r="M8">
-        <v>-0.46</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -782,37 +782,37 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>-0.55000000000000004</v>
+        <v>-0.74</v>
       </c>
       <c r="D9">
-        <v>-0.46</v>
+        <v>-0.52</v>
       </c>
       <c r="E9">
-        <v>-0.62</v>
+        <v>-0.77</v>
       </c>
       <c r="F9">
-        <v>-1.46</v>
+        <v>-0.54</v>
       </c>
       <c r="G9">
-        <v>-0.53</v>
+        <v>-0.47</v>
       </c>
       <c r="H9">
-        <v>0.06</v>
+        <v>-0.31</v>
       </c>
       <c r="I9">
-        <v>-0.65</v>
+        <v>-1.07</v>
       </c>
       <c r="J9">
-        <v>-0.55000000000000004</v>
+        <v>-0.94</v>
       </c>
       <c r="K9">
-        <v>-0.23</v>
+        <v>-0.35</v>
       </c>
       <c r="L9">
-        <v>-0.83</v>
+        <v>-0.61</v>
       </c>
       <c r="M9">
-        <v>-0.46</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -823,37 +823,37 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>-0.24</v>
+        <v>-0.66</v>
       </c>
       <c r="D10">
-        <v>0.31</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="E10">
-        <v>-1.58</v>
+        <v>-0.42</v>
       </c>
       <c r="F10">
-        <v>0.45</v>
+        <v>-0.22</v>
       </c>
       <c r="G10">
-        <v>0.06</v>
+        <v>-0.25</v>
       </c>
       <c r="H10">
-        <v>0.13</v>
+        <v>-0.42</v>
       </c>
       <c r="I10">
-        <v>0.28999999999999998</v>
+        <v>-0.36</v>
       </c>
       <c r="J10">
-        <v>0.34</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="K10">
-        <v>-0.09</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="L10">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="M10">
-        <v>0.36</v>
+        <v>-0.28999999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -862,37 +862,37 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>-0.24</v>
+        <v>-0.6</v>
       </c>
       <c r="D11">
-        <v>0.27</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="E11">
-        <v>-1.59</v>
+        <v>-0.41</v>
       </c>
       <c r="F11">
-        <v>0.46</v>
+        <v>-0.17</v>
       </c>
       <c r="G11">
-        <v>0.05</v>
+        <v>-0.25</v>
       </c>
       <c r="H11">
-        <v>0.13</v>
+        <v>-0.43</v>
       </c>
       <c r="I11">
-        <v>0.33</v>
+        <v>-0.31</v>
       </c>
       <c r="J11">
-        <v>0.37</v>
+        <v>-0.25</v>
       </c>
       <c r="K11">
-        <v>-0.12</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="L11">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="M11">
-        <v>0.39</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -901,37 +901,37 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>-0.24</v>
+        <v>-0.6</v>
       </c>
       <c r="D12">
-        <v>0.25</v>
+        <v>-0.3</v>
       </c>
       <c r="E12">
-        <v>-1.59</v>
+        <v>-0.41</v>
       </c>
       <c r="F12">
-        <v>0.47</v>
+        <v>-0.17</v>
       </c>
       <c r="G12">
-        <v>0.03</v>
+        <v>-0.26</v>
       </c>
       <c r="H12">
-        <v>0.13</v>
+        <v>-0.43</v>
       </c>
       <c r="I12">
-        <v>0.34</v>
+        <v>-0.31</v>
       </c>
       <c r="J12">
-        <v>0.38</v>
+        <v>-0.25</v>
       </c>
       <c r="K12">
-        <v>-0.12</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="L12">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="M12">
-        <v>0.39</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -940,37 +940,37 @@
         <v>15</v>
       </c>
       <c r="C13">
+        <v>-0.61</v>
+      </c>
+      <c r="D13">
+        <v>-0.3</v>
+      </c>
+      <c r="E13">
+        <v>-0.42</v>
+      </c>
+      <c r="F13">
+        <v>-0.16</v>
+      </c>
+      <c r="G13">
+        <v>-0.26</v>
+      </c>
+      <c r="H13">
+        <v>-0.43</v>
+      </c>
+      <c r="I13">
+        <v>-0.31</v>
+      </c>
+      <c r="J13">
         <v>-0.24</v>
       </c>
-      <c r="D13">
-        <v>0.22</v>
-      </c>
-      <c r="E13">
-        <v>-1.59</v>
-      </c>
-      <c r="F13">
-        <v>0.47</v>
-      </c>
-      <c r="G13">
-        <v>-0.01</v>
-      </c>
-      <c r="H13">
-        <v>0.13</v>
-      </c>
-      <c r="I13">
-        <v>0.35</v>
-      </c>
-      <c r="J13">
-        <v>0.38</v>
-      </c>
       <c r="K13">
-        <v>-0.13</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="L13">
-        <v>-0.39</v>
+        <v>-0.37</v>
       </c>
       <c r="M13">
-        <v>0.39</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -981,37 +981,37 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-0.32</v>
+        <v>-0.71</v>
       </c>
       <c r="D14">
-        <v>0.2</v>
+        <v>-0.35</v>
       </c>
       <c r="E14">
-        <v>-2.14</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="F14">
-        <v>-2.0099999999999998</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="G14">
-        <v>-0.28000000000000003</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="H14">
-        <v>0.19</v>
+        <v>-0.33</v>
       </c>
       <c r="I14">
-        <v>-0.12</v>
+        <v>-0.67</v>
       </c>
       <c r="J14">
-        <v>-0.3</v>
+        <v>-0.62</v>
       </c>
       <c r="K14">
-        <v>-0.01</v>
+        <v>-0.49</v>
       </c>
       <c r="L14">
-        <v>-0.56000000000000005</v>
+        <v>-0.45</v>
       </c>
       <c r="M14">
-        <v>-0.2</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1020,37 +1020,37 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>-0.27</v>
+        <v>-1.41</v>
       </c>
       <c r="D15">
-        <v>0.19</v>
+        <v>-0.33</v>
       </c>
       <c r="E15">
-        <v>-2.12</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="F15">
-        <v>-2.29</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="G15">
-        <v>-11883354.07</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="H15">
-        <v>-350819.04</v>
+        <v>-0.33</v>
       </c>
       <c r="I15">
-        <v>-0.12</v>
+        <v>-0.67</v>
       </c>
       <c r="J15">
-        <v>-0.3</v>
+        <v>-0.62</v>
       </c>
       <c r="K15">
-        <v>-0.01</v>
+        <v>-0.49</v>
       </c>
       <c r="L15">
-        <v>-0.56000000000000005</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="M15">
-        <v>-0.2</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1059,37 +1059,37 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>-0.27</v>
+        <v>-1.1599999999999999</v>
       </c>
       <c r="D16">
-        <v>0.18</v>
+        <v>-0.33</v>
       </c>
       <c r="E16">
-        <v>-2.06</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="F16">
-        <v>-2.6</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="G16">
-        <v>-52534948.799999997</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="H16">
-        <v>-1182358.04</v>
+        <v>-0.33</v>
       </c>
       <c r="I16">
-        <v>-0.12</v>
+        <v>-0.67</v>
       </c>
       <c r="J16">
-        <v>-0.3</v>
+        <v>-0.62</v>
       </c>
       <c r="K16">
-        <v>-0.01</v>
+        <v>-0.49</v>
       </c>
       <c r="L16">
-        <v>-0.56000000000000005</v>
+        <v>-0.5</v>
       </c>
       <c r="M16">
-        <v>-0.2</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1098,37 +1098,37 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>-0.27</v>
+        <v>-0.71</v>
       </c>
       <c r="D17">
-        <v>0.17</v>
+        <v>-0.32</v>
       </c>
       <c r="E17">
-        <v>-2.14</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="F17">
-        <v>-3.4</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="G17">
-        <v>-315880791.11000001</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="H17">
-        <v>-3282813.07</v>
+        <v>-0.33</v>
       </c>
       <c r="I17">
-        <v>-0.12</v>
+        <v>-0.67</v>
       </c>
       <c r="J17">
-        <v>-0.3</v>
+        <v>-0.62</v>
       </c>
       <c r="K17">
-        <v>-0.01</v>
+        <v>-0.49</v>
       </c>
       <c r="L17">
-        <v>-0.56000000000000005</v>
+        <v>-0.49</v>
       </c>
       <c r="M17">
-        <v>-0.19</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1136,37 +1136,37 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-0.41</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-0.16</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-0.31</v>
+      </c>
+      <c r="J18" s="2">
         <v>-0.24</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-0.12</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.38</v>
-      </c>
       <c r="K18" s="2">
-        <v>-0.01</v>
+        <v>-0.34</v>
       </c>
       <c r="L18" s="2">
-        <v>-0.16</v>
+        <v>-0.37</v>
       </c>
       <c r="M18" s="2">
-        <v>0.39</v>
+        <v>-0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>